<commit_message>
19 Feb 2025 Part 3
</commit_message>
<xml_diff>
--- a/automate/Projects.xlsx
+++ b/automate/Projects.xlsx
@@ -12,24 +12,28 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Projects</t>
+  </si>
   <si>
     <t>awais.hamid@ascend.com.sa</t>
   </si>
   <si>
-    <t>Holidays  /  Annual Leaves</t>
+    <t>Waiting for approval</t>
   </si>
   <si>
-    <t>NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing</t>
-  </si>
-  <si>
-    <t>Asset Performance Management  /  Implementation and Support</t>
-  </si>
-  <si>
-    <t>MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection</t>
-  </si>
-  <si>
-    <t>N/A - Digital Innovation-Investment Work-Non-PO  /  efficonX</t>
+    <t>Holidays  /  Annual Leaves
+NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing
+Asset Performance Management  /  Implementation and Support
+MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection
+N/A - Digital Innovation-Investment Work-Non-PO  /  efficonX</t>
   </si>
 </sst>
 </file>
@@ -66,19 +70,27 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment wrapText="true"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
+  <cols>
+    <col min="1" max="1" width="27.35546875" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="19.42578125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="65.9375" customWidth="true" bestFit="true"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="s" s="0">
@@ -87,36 +99,18 @@
       <c r="B1" t="s" s="0">
         <v>1</v>
       </c>
+      <c r="C1" t="s" s="0">
+        <v>2</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s" s="0">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B3" t="s" s="0">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B5" t="s" s="0">
+      <c r="C2" t="s" s="1">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
20 Feb 2025 Part 1
</commit_message>
<xml_diff>
--- a/automate/Projects.xlsx
+++ b/automate/Projects.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Email</t>
   </si>
@@ -34,6 +34,16 @@
 Asset Performance Management  /  Implementation and Support
 MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection
 N/A - Digital Innovation-Investment Work-Non-PO  /  efficonX</t>
+  </si>
+  <si>
+    <t>romeesa.ashfaq@ascend.com.sa</t>
+  </si>
+  <si>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>MoH Compliance Program_Digital  /  Others (QA)
+MoH Compliance Program_Digital  /  Others (dotnet)</t>
   </si>
 </sst>
 </file>
@@ -81,13 +91,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="27.35546875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="30.421875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="19.42578125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="65.9375" customWidth="true" bestFit="true"/>
   </cols>
@@ -114,6 +124,17 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s" s="0">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s" s="1">
+        <v>8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
23 Feb 2025 Part 1
</commit_message>
<xml_diff>
--- a/automate/Projects.xlsx
+++ b/automate/Projects.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
   <si>
     <t>Name</t>
   </si>
@@ -29,30 +29,32 @@
     <t>Waiting for approval</t>
   </si>
   <si>
-    <t>Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Others (docker security and build automation)
-NUPCO Command Centre  /  Others (On prem deployment fixes)</t>
+    <t>Support for ASCEND Operation  /  Others (dev migration to huawei cloud)
+Support for ASCEND Operation  /  Others (tech support to dev teams on floor)</t>
   </si>
   <si>
     <t>muhammad.ilyas@ascend.com.sa</t>
   </si>
   <si>
-    <t>MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection</t>
+    <t>Approved</t>
+  </si>
+  <si>
+    <t>MoH Compliance Program_Digital  /  No Tasks</t>
   </si>
   <si>
     <t>hassan.shafique@ascend.com.sa</t>
   </si>
   <si>
+    <t>MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection
+PC2264 - NHCC_3.0_Digital Products  /  No Tasks
+MoH Compliance Program_Digital  /  Others (dot net micro services)
+PC2264 - NHCC_3.0_Digital Products  /  Others (Agentive AI)</t>
+  </si>
+  <si>
+    <t>awais.hamid@ascend.com.sa</t>
+  </si>
+  <si>
     <t>NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing
-MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection
-Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - ELA - Ticketing
-MoH Compliance Program_Digital  /  Others (Dot Net Development)</t>
-  </si>
-  <si>
-    <t>awais.hamid@ascend.com.sa</t>
-  </si>
-  <si>
-    <t>Holidays  /  Annual Leaves
-NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing
 Asset Performance Management  /  Implementation and Support
 MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection
 N/A - Digital Innovation-Investment Work-Non-PO  /  efficonX</t>
@@ -61,14 +63,14 @@
     <t>parth.bhuta@ascend.com.sa</t>
   </si>
   <si>
-    <t>Approved</t>
-  </si>
-  <si>
-    <t>N/A - Digital Innovation-Investment Work-Non-PO  /  SharePoint Tasks
-N/A - Digital Innovation-Investment Work-Non-PO  /  SharePoint Tasks
-N/A - Digital Innovation-Investment Work-Non-PO  /  SharePoint Tasks
-N/A - Digital Innovation-Investment Work-Non-PO  /  SharePoint Tasks
-N/A - Digital Innovation-Investment Work-Non-PO  /  SharePoint Tasks</t>
+    <t>Not Submitted</t>
+  </si>
+  <si>
+    <t>N/A - Digital Innovation-Investment Work-Non-PO/SharePoint Tasks
+N/A - Digital Innovation-Investment Work-Non-PO/SharePoint Tasks
+N/A - Digital Innovation-Investment Work-Non-PO/SharePoint Tasks
+N/A - Digital Innovation-Investment Work-Non-PO/SharePoint Tasks
+N/A - Digital Innovation-Investment Work-Non-PO/SharePoint Tasks</t>
   </si>
   <si>
     <t>faesal.alacher@ascend.com.sa</t>
@@ -82,10 +84,9 @@
     <t>anas.yassin@ascend.com.sa</t>
   </si>
   <si>
-    <t>N/A - Digital Innovation-Investment Work-Non-PO  /  Astrom (NEC-MOHU-Others)
-N/A - Digital Innovation-Investment Work-Non-PO  /  EfficaX Zairoon - MOH Visiting Doctor
-N/A - Digital Innovation-Investment Work-Non-PO  /  Product Development RnD
-Holidays  /  Annual Leaves</t>
+    <t>N/A - Digital Innovation-Investment Work-Non-PO  /  EfficaX Zairoon - MOH Visiting Doctor
+N/A - Digital Innovation-Investment Work-Non-PO  /  Astrom (NEC-MOHU-Others)
+N/A - Digital Innovation-Investment Work-Non-PO  /  Product Development RnD</t>
   </si>
   <si>
     <t>awad.warag@ascend.com.sa</t>
@@ -97,34 +98,29 @@
     <t>mohsin.ali@ascend.com.sa</t>
   </si>
   <si>
-    <t>Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - RPA - UiPath
-Hajj &amp; Umrah Command Center_PMO  /  Others (Data Engineering)</t>
+    <t>Hajj &amp; Umrah Command Center_PMO  /  Others (Data Engineering)</t>
   </si>
   <si>
     <t>ziad.safa@ascend.com.sa</t>
   </si>
   <si>
-    <t>Not Submitted</t>
+    <t>Asset Performance Management  /  Project Management
+Taakad Gen - II  /  PMO
+Asset Performance Management  /  Project Management</t>
+  </si>
+  <si>
+    <t>haneen.aseeri@ascend.com.sa</t>
+  </si>
+  <si>
+    <t>PC2264 - NHCC_3.0_Digital Products  /  No Tasks</t>
+  </si>
+  <si>
+    <t>danial.ghazali@ascend.com.sa</t>
   </si>
   <si>
     <t>No Project/No Tasks</t>
   </si>
   <si>
-    <t>haneen.aseeri@ascend.com.sa</t>
-  </si>
-  <si>
-    <t>NHCC_3.0_Consulting  /  No Tasks</t>
-  </si>
-  <si>
-    <t>danial.ghazali@ascend.com.sa</t>
-  </si>
-  <si>
-    <t>Hajj &amp; Umrah Command Center_PMO/Others
-NUPCO Command Centre/Digital / Ticketing
-Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh/Digital Innovation - ELA - Ticketing
-NHCC_3.0_Consulting/Digital Innovation - ELA - Ticketing</t>
-  </si>
-  <si>
     <t>abeer.alatabani@ascend.com.sa</t>
   </si>
   <si>
@@ -135,8 +131,8 @@
   </si>
   <si>
     <t>NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing
-Asset Performance Management  /  Others (Design)
-N/A - Digital Innovation-Investment Work-Non-PO  /  Creative Design</t>
+N/A - Digital Innovation-Investment Work-Non-PO  /  Creative Design
+Holidays  /  Sick Leave</t>
   </si>
   <si>
     <t>bilal.ahmed@ascend.com.sa</t>
@@ -149,8 +145,10 @@
     <t>hassan.javed@ascend.com.sa</t>
   </si>
   <si>
-    <t>NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing
-Business Development  /  Commercial Development</t>
+    <t>Business Development  /  Business Development Activities
+N/A - Digital Innovation-Investment Work-Non-PO  /  Ascend Events (PAJ, XLR8, LIV)
+MoH Compliance Program_Digital  /  Project Management
+Self Development  /  Self Development</t>
   </si>
   <si>
     <t>sajjad.haider@ascend.com.sa</t>
@@ -162,28 +160,31 @@
     <t>zeeshan.ali@ascend.com.sa</t>
   </si>
   <si>
-    <t>Professional Services to Implement Data Office in SCFHS  /  Others (Deliverables)</t>
+    <t>Professional Services to Implement Data Office in SCFHS  /  Others (FOI Delivery Tasks)</t>
   </si>
   <si>
     <t>masub.imtiaz@ascend.com.sa</t>
   </si>
   <si>
-    <t>MoH Compliance Program_Digital  /  No Tasks</t>
-  </si>
-  <si>
     <t>abdulahad.tahir@ascend.com.sa</t>
   </si>
   <si>
+    <t>MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection</t>
+  </si>
+  <si>
     <t>hassan.aamir@ascend.com.sa</t>
   </si>
   <si>
+    <t>PC2264 - NHCC_3.0_Digital Products  /  Others</t>
+  </si>
+  <si>
+    <t>haseeb.mukhtar@ascend.com.sa</t>
+  </si>
+  <si>
+    <t>shoaib.atiq@ascend.com.sa</t>
+  </si>
+  <si>
     <t>NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing</t>
-  </si>
-  <si>
-    <t>haseeb.mukhtar@ascend.com.sa</t>
-  </si>
-  <si>
-    <t>shoaib.atiq@ascend.com.sa</t>
   </si>
   <si>
     <t>hamayun.khan@ascend.com.sa</t>
@@ -226,6 +227,9 @@
     <t>muhammad.usman@ascend.com.sa</t>
   </si>
   <si>
+    <t>abdul.mannan@ascend.com.sa</t>
+  </si>
+  <si>
     <t>rizwan.ali@ascend.com.sa</t>
   </si>
   <si>
@@ -233,24 +237,24 @@
   </si>
   <si>
     <t>Other Internal Tasks  /  Others (migration)
-Support for ASCEND Operation  /  Others (chi-on-prem setup)
+Support for ASCEND Operation  /  Others (dev teams task)
 Other Internal Tasks  /  Others (migration)
-Support for ASCEND Operation  /  Others (dev teams task)
-Support for ASCEND Operation  /  Others (migration)
-Other Internal Tasks  /  Others (dev teams collaboration)
-Support for ASCEND Operation  /  Others (migration)
-Support for ASCEND Operation  /  Others (astrum prod issue)
-Other Internal Tasks  /  Others (dev teams collaboration)
-Support for ASCEND Operation  /  Others (migration)
-Other Internal Tasks  /  Others (dev team collaboration)
-Other Internal Tasks  /  Others (dev-collaboration)</t>
+Support for ASCEND Operation  /  Others (dev-team task)
+Support for ASCEND Operation  /  Others (astrum dbs issue)
+Other Internal Tasks  /  Others (migration)
+Support for ASCEND Operation  /  Others (dev-team support)
+Other Internal Tasks  /  Others (migration)
+Support for ASCEND Operation  /  Others (dev-teams task)
+Other Internal Tasks  /  Others (dev-teams task)
+Self Development  /  Self Development</t>
   </si>
   <si>
     <t>safwan.asghar@ascend.com.sa</t>
   </si>
   <si>
     <t>Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - RPA - UiPath
-Hajj &amp; Umrah Command Center_PMO  /  Others (Ticketing)</t>
+Hajj &amp; Umrah Command Center_PMO  /  Others (Ticketing)
+NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing</t>
   </si>
   <si>
     <t>muhammad.umair@ascend.com.sa</t>
@@ -265,23 +269,25 @@
     <t>salman.nishan@ascend.com.sa</t>
   </si>
   <si>
-    <t>NUPCO Command Centre  /  Digital / Ticketing</t>
+    <t>NUPCO Command Centre  /  Digital / Ticketing
+MoH Compliance Program_Digital  /  Data Analytics
+Holidays  /  Sick Leave</t>
   </si>
   <si>
     <t>basel.makhdoum@ascend.com.sa</t>
   </si>
   <si>
     <t>Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - ELA - Ticketing
-Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - RPA - UiPath</t>
+Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - RPA - UiPath
+Holidays  /  Annual Leaves</t>
   </si>
   <si>
     <t>athar.ali@ascend.com.sa</t>
   </si>
   <si>
     <t>NHCC_3.0_Consulting  /  Digital Innovation - ELA - Ticketing
-NHCC_3.0_Consulting  /  Others (Illustration)
 MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection
-Holidays  /  Others</t>
+Holidays  /  Casual Leave</t>
   </si>
   <si>
     <t>khadija.yasin@ascend.com.sa</t>
@@ -291,14 +297,10 @@
   </si>
   <si>
     <t>MoH Compliance Program_Digital  /  Others (QA)
-MoH Compliance Program_Digital  /  Others (dotnet)</t>
+MoH Compliance Program_Digital  /  Others (SCoc)</t>
   </si>
   <si>
     <t>rida.khan@ascend.com.sa</t>
-  </si>
-  <si>
-    <t>NHCC_3.0_Consulting  /  Others (Support)
-MoH Compliance Program_Digital  /  Others (Taftesh)</t>
   </si>
   <si>
     <t>mudassar.iqbal@ascend.com.sa</t>
@@ -352,7 +354,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C46"/>
+  <dimension ref="A1:C47"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -360,7 +362,7 @@
   <cols>
     <col min="1" max="1" width="34.390625" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="19.42578125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="111.00390625" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="100.81640625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -390,95 +392,95 @@
         <v>6</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s" s="0">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C4" t="s" s="1">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s" s="1">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s" s="1">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s" s="1">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C8" t="s" s="1">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C9" t="s" s="1">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B10" t="s" s="0">
         <v>4</v>
       </c>
       <c r="C10" t="s" s="1">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="C11" t="s" s="1">
         <v>25</v>
@@ -489,7 +491,7 @@
         <v>26</v>
       </c>
       <c r="B12" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C12" t="s" s="1">
         <v>27</v>
@@ -500,7 +502,7 @@
         <v>28</v>
       </c>
       <c r="B13" t="s" s="0">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s" s="1">
         <v>29</v>
@@ -522,7 +524,7 @@
         <v>32</v>
       </c>
       <c r="B15" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C15" t="s" s="1">
         <v>33</v>
@@ -533,7 +535,7 @@
         <v>34</v>
       </c>
       <c r="B16" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C16" t="s" s="1">
         <v>35</v>
@@ -544,7 +546,7 @@
         <v>36</v>
       </c>
       <c r="B17" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s" s="1">
         <v>37</v>
@@ -555,7 +557,7 @@
         <v>38</v>
       </c>
       <c r="B18" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C18" t="s" s="1">
         <v>39</v>
@@ -566,7 +568,7 @@
         <v>40</v>
       </c>
       <c r="B19" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s" s="1">
         <v>41</v>
@@ -577,21 +579,21 @@
         <v>42</v>
       </c>
       <c r="B20" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C20" t="s" s="1">
-        <v>43</v>
+        <v>8</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B21" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C21" t="s" s="1">
         <v>44</v>
-      </c>
-      <c r="B21" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s" s="1">
-        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -610,10 +612,10 @@
         <v>47</v>
       </c>
       <c r="B23" t="s" s="0">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="C23" t="s" s="1">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="24">
@@ -621,142 +623,142 @@
         <v>48</v>
       </c>
       <c r="B24" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s" s="1">
-        <v>46</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B25" t="s" s="0">
-        <v>24</v>
+        <v>14</v>
       </c>
       <c r="C25" t="s" s="1">
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B26" t="s" s="0">
-        <v>4</v>
+        <v>14</v>
       </c>
       <c r="C26" t="s" s="1">
-        <v>46</v>
+        <v>29</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B27" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s" s="1">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B28" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s" s="1">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B29" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s" s="1">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B30" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s" s="1">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B31" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s" s="1">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B32" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s" s="1">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s" s="0">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B33" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s" s="1">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s" s="0">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B34" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s" s="1">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="0">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B35" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s" s="1">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s" s="0">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B36" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s" s="1">
-        <v>64</v>
+        <v>44</v>
       </c>
     </row>
     <row r="37">
@@ -764,7 +766,7 @@
         <v>65</v>
       </c>
       <c r="B37" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C37" t="s" s="1">
         <v>66</v>
@@ -775,7 +777,7 @@
         <v>67</v>
       </c>
       <c r="B38" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s" s="1">
         <v>68</v>
@@ -786,21 +788,21 @@
         <v>69</v>
       </c>
       <c r="B39" t="s" s="0">
-        <v>24</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s" s="1">
-        <v>25</v>
+        <v>70</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s" s="0">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B40" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s" s="1">
-        <v>71</v>
+        <v>29</v>
       </c>
     </row>
     <row r="41">
@@ -808,7 +810,7 @@
         <v>72</v>
       </c>
       <c r="B41" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C41" t="s" s="1">
         <v>73</v>
@@ -819,7 +821,7 @@
         <v>74</v>
       </c>
       <c r="B42" t="s" s="0">
-        <v>13</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s" s="1">
         <v>75</v>
@@ -830,21 +832,21 @@
         <v>76</v>
       </c>
       <c r="B43" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C43" t="s" s="1">
-        <v>46</v>
+        <v>77</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="0">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B44" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C44" t="s" s="1">
-        <v>78</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45">
@@ -852,7 +854,7 @@
         <v>79</v>
       </c>
       <c r="B45" t="s" s="0">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C45" t="s" s="1">
         <v>80</v>
@@ -863,10 +865,21 @@
         <v>81</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C46" t="s" s="1">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s" s="0">
         <v>82</v>
+      </c>
+      <c r="B47" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C47" t="s" s="1">
+        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24 Feb 2025 Part 1
</commit_message>
<xml_diff>
--- a/automate/Projects.xlsx
+++ b/automate/Projects.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -280,6 +280,14 @@
     <t>Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - ELA - Ticketing
 Council of Health Insurance_Integrated Intelligence and AI Center_Riyadh  /  Digital Innovation - RPA - UiPath
 Holidays  /  Annual Leaves</t>
+  </si>
+  <si>
+    <t>zuhran.ahmed@ascend.com.sa</t>
+  </si>
+  <si>
+    <t>MoH Compliance Program_Digital  /  Digital Innovation - EFX - Inspection
+N/A - Digital Innovation-Investment Work-Non-PO  /  Astrom (NEC-MOHU-Others)
+N/A - Digital Innovation-Investment Work-Non-PO  /  No Tasks</t>
   </si>
   <si>
     <t>athar.ali@ascend.com.sa</t>
@@ -354,7 +362,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C47"/>
+  <dimension ref="A1:C48"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -846,18 +854,18 @@
         <v>7</v>
       </c>
       <c r="C44" t="s" s="1">
-        <v>49</v>
+        <v>79</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="0">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B45" t="s" s="0">
         <v>7</v>
       </c>
       <c r="C45" t="s" s="1">
-        <v>80</v>
+        <v>49</v>
       </c>
     </row>
     <row r="46">
@@ -865,21 +873,32 @@
         <v>81</v>
       </c>
       <c r="B46" t="s" s="0">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s" s="1">
-        <v>29</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s" s="0">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s" s="0">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C47" t="s" s="1">
-        <v>83</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s" s="0">
+        <v>84</v>
+      </c>
+      <c r="B48" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C48" t="s" s="1">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>